<commit_message>
Started work on CurtainControl
</commit_message>
<xml_diff>
--- a/Bill of Materials.xlsx
+++ b/Bill of Materials.xlsx
@@ -595,7 +595,7 @@
   <dimension ref="A1:L360"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,14 +684,14 @@
       </c>
       <c r="B4" s="10">
         <f>H4/G4</f>
-        <v>4.6100000000000003</v>
+        <v>3</v>
       </c>
       <c r="C4" s="9">
         <v>1</v>
       </c>
       <c r="D4" s="10">
         <f>C4*B4</f>
-        <v>4.6100000000000003</v>
+        <v>3</v>
       </c>
       <c r="E4" s="14">
         <f>C4*$L$6</f>
@@ -699,13 +699,13 @@
       </c>
       <c r="F4" s="10">
         <f>E4*B4</f>
-        <v>9.2200000000000006</v>
+        <v>6</v>
       </c>
       <c r="G4" s="9">
         <v>1</v>
       </c>
       <c r="H4" s="12">
-        <v>4.6100000000000003</v>
+        <v>3</v>
       </c>
       <c r="I4" s="1">
         <f>_xlfn.CEILING.MATH(E4/G4)</f>
@@ -713,15 +713,15 @@
       </c>
       <c r="J4" s="11">
         <f>I4*H4</f>
-        <v>9.2200000000000006</v>
+        <v>6</v>
       </c>
       <c r="K4" s="13">
         <f>SUM(D4:D47)</f>
-        <v>15.481800000000003</v>
+        <v>13.8718</v>
       </c>
       <c r="L4" s="13">
         <f>SUM(J4:J46) + L5</f>
-        <v>47.06</v>
+        <v>43.84</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -854,7 +854,7 @@
       </c>
       <c r="L7" s="15">
         <f>L4/L6</f>
-        <v>23.53</v>
+        <v>21.92</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>